<commit_message>
Gene family file parser updates
- Null files for SEQ data that are all NULL, and when a malformed Newick tree is provided
- Output newick tree with leaves labeled as common name, scientific name, gene, and protein ID (default)
- Minor changes and fixes
</commit_message>
<xml_diff>
--- a/speciesNameConverter.xlsx
+++ b/speciesNameConverter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GitHub\MolecularEvolutionFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EF87B9-132B-403B-A5BA-04B23BF74AC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB78A9-4988-4E0B-874F-905A68CFAD03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C6F7853B-798C-4B33-8020-EDB0E69493D0}"/>
+    <workbookView xWindow="0" yWindow="4530" windowWidth="38400" windowHeight="18390" xr2:uid="{C6F7853B-798C-4B33-8020-EDB0E69493D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -261,9 +261,6 @@
     <t>aotus_nancymaae</t>
   </si>
   <si>
-    <t>ma's_night_monkey</t>
-  </si>
-  <si>
     <t>ENSANA</t>
   </si>
   <si>
@@ -468,9 +465,6 @@
     <t>choloepus_hoffmanni</t>
   </si>
   <si>
-    <t>Hoffmann's_two_fingered_sloth</t>
-  </si>
-  <si>
     <t>ENSCHO</t>
   </si>
   <si>
@@ -508,6 +502,12 @@
   </si>
   <si>
     <t>ENSETEP</t>
+  </si>
+  <si>
+    <t>mas_night_monkey</t>
+  </si>
+  <si>
+    <t>Hoffmanns_two_fingered_sloth</t>
   </si>
 </sst>
 </file>
@@ -861,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12AFC2D-F2F6-4AE5-A17F-9710BBEC3751}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,307 +1152,307 @@
         <v>74</v>
       </c>
       <c r="B26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>81</v>
-      </c>
-      <c r="C28" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>84</v>
-      </c>
-      <c r="C29" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
         <v>86</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>87</v>
-      </c>
-      <c r="C30" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
         <v>89</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>90</v>
-      </c>
-      <c r="C31" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
         <v>92</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>93</v>
-      </c>
-      <c r="C32" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
         <v>95</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>96</v>
-      </c>
-      <c r="C33" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" t="s">
         <v>98</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>99</v>
-      </c>
-      <c r="C34" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" t="s">
         <v>101</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>102</v>
-      </c>
-      <c r="C35" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
         <v>104</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>105</v>
-      </c>
-      <c r="C36" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
         <v>107</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>108</v>
-      </c>
-      <c r="C37" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" t="s">
         <v>110</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>111</v>
-      </c>
-      <c r="C38" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" t="s">
         <v>113</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>114</v>
-      </c>
-      <c r="C39" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" t="s">
         <v>116</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>117</v>
-      </c>
-      <c r="C40" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" t="s">
         <v>119</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>120</v>
-      </c>
-      <c r="C41" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" t="s">
         <v>122</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>123</v>
-      </c>
-      <c r="C42" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" t="s">
         <v>125</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>126</v>
-      </c>
-      <c r="C43" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" t="s">
         <v>128</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>129</v>
-      </c>
-      <c r="C44" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" t="s">
         <v>131</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>132</v>
-      </c>
-      <c r="C45" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
         <v>134</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>135</v>
-      </c>
-      <c r="C46" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" t="s">
         <v>137</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>138</v>
-      </c>
-      <c r="C47" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" t="s">
         <v>140</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>141</v>
-      </c>
-      <c r="C48" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" t="s">
         <v>143</v>
-      </c>
-      <c r="B49" t="s">
-        <v>144</v>
-      </c>
-      <c r="C49" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" t="s">
         <v>146</v>
-      </c>
-      <c r="B50" t="s">
-        <v>147</v>
-      </c>
-      <c r="C50" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>147</v>
+      </c>
+      <c r="B51" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" t="s">
         <v>149</v>
-      </c>
-      <c r="B51" t="s">
-        <v>150</v>
-      </c>
-      <c r="C51" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" t="s">
         <v>152</v>
-      </c>
-      <c r="B52" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>153</v>
+      </c>
+      <c r="B53" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" t="s">
         <v>155</v>
-      </c>
-      <c r="B53" t="s">
-        <v>156</v>
-      </c>
-      <c r="C53" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>